<commit_message>
Finalisation MLD - Création du projet sur visual studio
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Projet programmation\Chat Application\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Projet programmation\Chat\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Personne</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Il y a une "incohérence" dans mes modèles: il faut que je trouve une meilleure facon de gérer les discussions (messages, membres)</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Front end</t>
+  </si>
+  <si>
+    <t>Page de connexion et 1ere page d'enregistrement</t>
   </si>
 </sst>
 </file>
@@ -733,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1022,19 +1031,35 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="5">
+        <v>43143</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="F17" s="30"/>
       <c r="G17" s="31"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="29"/>
+      <c r="B18" s="5">
+        <v>43143</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>41</v>
+      </c>
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
     </row>
@@ -1390,16 +1415,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1412,28 +1449,16 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MCD/MLD - Front end
La moitié du front end est réalisé. Les mcd et mld ont été corrigés
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Personne</t>
   </si>
@@ -150,6 +150,21 @@
   </si>
   <si>
     <t>Page de connexion et 1ere page d'enregistrement</t>
+  </si>
+  <si>
+    <t>MLD/MCD</t>
+  </si>
+  <si>
+    <t>20min</t>
+  </si>
+  <si>
+    <t>Corrections</t>
+  </si>
+  <si>
+    <t>70min</t>
+  </si>
+  <si>
+    <t>Moitié front end fait</t>
   </si>
 </sst>
 </file>
@@ -743,7 +758,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E20" sqref="E20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1065,19 +1080,35 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="5">
+        <v>43144</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="29"/>
+      <c r="B20" s="5">
+        <v>43144</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>46</v>
+      </c>
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
     </row>
@@ -1415,16 +1446,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="E25:G25"/>
@@ -1437,28 +1480,16 @@
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MLD- diagramme de classe
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>Personne</t>
   </si>
@@ -165,6 +165,21 @@
   </si>
   <si>
     <t>Moitié front end fait</t>
+  </si>
+  <si>
+    <t>terminé</t>
+  </si>
+  <si>
+    <t>Revu MLD prof</t>
+  </si>
+  <si>
+    <t>Modifications à apporter et réflechir sur "répondre à un user précis dans un groupe"</t>
+  </si>
+  <si>
+    <t>Documentation projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagramme de classe </t>
   </si>
 </sst>
 </file>
@@ -758,7 +773,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:G20"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1114,46 +1129,80 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="5">
+        <v>43146</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>47</v>
+      </c>
       <c r="F21" s="30"/>
       <c r="G21" s="31"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="23"/>
+      <c r="B22" s="5">
+        <v>43146</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E22" s="29"/>
       <c r="F22" s="30"/>
       <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="23"/>
+      <c r="B23" s="5">
+        <v>43146</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E23" s="29"/>
       <c r="F23" s="30"/>
       <c r="G23" s="31"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="23"/>
+      <c r="B24" s="5">
+        <v>43146</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="E24" s="29"/>
       <c r="F24" s="30"/>
       <c r="G24" s="31"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="29"/>
+      <c r="B25" s="5">
+        <v>43146</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>49</v>
+      </c>
       <c r="F25" s="30"/>
       <c r="G25" s="31"/>
     </row>
@@ -1329,22 +1378,22 @@
       <c r="G44" s="31"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="31"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
@@ -1427,35 +1476,39 @@
       <c r="F55" s="28"/>
       <c r="G55" s="28"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
+    <row r="1048575" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A1048575" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A1048576" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="XFD1048576" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+  <mergeCells count="43">
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1468,28 +1521,16 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementation classe - connexion BD
En cours : méthode de vérification du pseudo existant
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>Personne</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>80min</t>
+  </si>
+  <si>
+    <t>Implémentation des classes sous visual studio</t>
+  </si>
+  <si>
+    <t>Connexion à la BD + méthode pour vérifier si le pseudo rentré est déjà existant</t>
+  </si>
+  <si>
+    <t>Réflexion sur les classes enfants de user</t>
+  </si>
+  <si>
+    <t>10min</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -495,6 +507,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,7 +794,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:G26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1227,29 +1242,43 @@
       <c r="F26" s="30"/>
       <c r="G26" s="31"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="23"/>
+      <c r="B27" s="5">
+        <v>43158</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="E27" s="29"/>
       <c r="F27" s="30"/>
       <c r="G27" s="31"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="23"/>
+      <c r="C28" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="E28" s="29"/>
       <c r="F28" s="30"/>
       <c r="G28" s="31"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="23"/>
+      <c r="C29" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E29" s="29"/>
       <c r="F29" s="30"/>
       <c r="G29" s="31"/>
@@ -1390,7 +1419,7 @@
       <c r="G44" s="31"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="7"/>
       <c r="C45" s="18"/>
       <c r="D45" s="24"/>
@@ -1399,7 +1428,7 @@
       <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="8"/>
       <c r="C46" s="19"/>
       <c r="D46" s="25"/>
@@ -1488,28 +1517,40 @@
       <c r="F55" s="28"/>
       <c r="G55" s="28"/>
     </row>
-    <row r="1048575" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A1048575" s="9" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+    </row>
+    <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A1048576" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
       <c r="XFD1048576" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1522,27 +1563,16 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implémentation Enregistrement + Connexion
.
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ProjetProgrammation\Chat\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12210" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Personne</t>
   </si>
@@ -216,12 +216,27 @@
   </si>
   <si>
     <t>Modification de la vérification du pseudo/mdp + ajout des données rentrées lors de l'enregistrement dans la base de données. MDP non crypté, photo non/mal traitée</t>
+  </si>
+  <si>
+    <t>29.02.2018</t>
+  </si>
+  <si>
+    <t>180min</t>
+  </si>
+  <si>
+    <t>Cryptage du mot de passe fonctionnel, la photo rentre dans la pictureBox et est enregistrée en local</t>
+  </si>
+  <si>
+    <t>Implémentation de la connexion</t>
+  </si>
+  <si>
+    <t>Vérification que les identifiants correspondent. Implémentation du bouton "remember me"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -508,6 +523,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -533,9 +551,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -817,11 +832,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -836,29 +851,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -874,11 +889,11 @@
       <c r="D4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -893,11 +908,11 @@
       <c r="D5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -912,11 +927,11 @@
       <c r="D6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -931,11 +946,11 @@
       <c r="D7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -950,11 +965,11 @@
       <c r="D8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -969,11 +984,11 @@
       <c r="D9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -988,11 +1003,11 @@
       <c r="D10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1007,11 +1022,11 @@
       <c r="D11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1029,11 +1044,11 @@
       <c r="D12" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -1048,11 +1063,11 @@
       <c r="D13" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1067,11 +1082,11 @@
       <c r="D14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
@@ -1084,11 +1099,11 @@
       <c r="D15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
@@ -1101,11 +1116,11 @@
       <c r="D16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
@@ -1118,11 +1133,11 @@
       <c r="D17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -1135,11 +1150,11 @@
       <c r="D18" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
@@ -1152,11 +1167,11 @@
       <c r="D19" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -1169,11 +1184,11 @@
       <c r="D20" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
@@ -1186,11 +1201,11 @@
       <c r="D21" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
@@ -1203,9 +1218,9 @@
       <c r="D22" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="32"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
@@ -1218,9 +1233,9 @@
       <c r="D23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="32"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
@@ -1233,9 +1248,9 @@
       <c r="D24" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -1248,11 +1263,11 @@
       <c r="D25" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
@@ -1265,9 +1280,9 @@
       <c r="D26" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
@@ -1280,9 +1295,9 @@
       <c r="D27" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="32"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
@@ -1293,9 +1308,9 @@
       <c r="D28" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
@@ -1306,12 +1321,12 @@
       <c r="D29" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="32"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="5">
@@ -1323,14 +1338,14 @@
       <c r="D30" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E30" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="5">
@@ -1342,128 +1357,142 @@
       <c r="D31" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="31"/>
-      <c r="G31" s="32"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="32"/>
+      <c r="G31" s="33"/>
+    </row>
+    <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
+    </row>
+    <row r="33" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="32"/>
+      <c r="C33" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="6"/>
       <c r="C34" s="17"/>
       <c r="D34" s="23"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="32"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="33"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="6"/>
       <c r="C35" s="17"/>
       <c r="D35" s="23"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="32"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="6"/>
       <c r="C36" s="17"/>
       <c r="D36" s="23"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="32"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="6"/>
       <c r="C37" s="17"/>
       <c r="D37" s="23"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="32"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="33"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="6"/>
       <c r="C38" s="17"/>
       <c r="D38" s="23"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="6"/>
       <c r="C39" s="17"/>
       <c r="D39" s="23"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="32"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="6"/>
       <c r="C40" s="17"/>
       <c r="D40" s="23"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="32"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="6"/>
       <c r="C41" s="17"/>
       <c r="D41" s="23"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="32"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="6"/>
       <c r="C42" s="17"/>
       <c r="D42" s="23"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="6"/>
       <c r="C43" s="17"/>
       <c r="D43" s="23"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="32"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="33"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="6"/>
       <c r="C44" s="17"/>
       <c r="D44" s="23"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="32"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="33"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
@@ -1577,16 +1606,27 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1599,27 +1639,16 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MonProfil - Affichage des informations
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
   <si>
     <t>Personne</t>
   </si>
@@ -231,6 +231,12 @@
   </si>
   <si>
     <t>Vérification que les identifiants correspondent. Implémentation du bouton "remember me"</t>
+  </si>
+  <si>
+    <t>CODE A NETTOYER</t>
+  </si>
+  <si>
+    <t>Lorsqu'on se connecte, les informations s'affichent sur notre profil</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -526,6 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -835,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -848,32 +855,33 @@
     <col min="5" max="5" width="9.5" style="26" customWidth="1"/>
     <col min="6" max="6" width="7.125" style="26" customWidth="1"/>
     <col min="7" max="7" width="24.125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -889,11 +897,11 @@
       <c r="D4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -908,11 +916,11 @@
       <c r="D5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -927,11 +935,11 @@
       <c r="D6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -946,11 +954,11 @@
       <c r="D7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -965,11 +973,11 @@
       <c r="D8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -984,11 +992,11 @@
       <c r="D9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1003,11 +1011,11 @@
       <c r="D10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1022,11 +1030,11 @@
       <c r="D11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1044,11 +1052,11 @@
       <c r="D12" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -1063,11 +1071,11 @@
       <c r="D13" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1082,11 +1090,11 @@
       <c r="D14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
@@ -1099,11 +1107,11 @@
       <c r="D15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
@@ -1116,11 +1124,11 @@
       <c r="D16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
@@ -1133,11 +1141,11 @@
       <c r="D17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -1150,11 +1158,11 @@
       <c r="D18" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
@@ -1167,11 +1175,11 @@
       <c r="D19" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -1184,11 +1192,11 @@
       <c r="D20" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
@@ -1201,11 +1209,11 @@
       <c r="D21" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="34"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
@@ -1218,9 +1226,9 @@
       <c r="D22" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
@@ -1233,9 +1241,9 @@
       <c r="D23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
@@ -1248,9 +1256,9 @@
       <c r="D24" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -1263,11 +1271,11 @@
       <c r="D25" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
@@ -1280,9 +1288,9 @@
       <c r="D26" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
@@ -1295,9 +1303,9 @@
       <c r="D27" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
@@ -1308,9 +1316,9 @@
       <c r="D28" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
@@ -1321,9 +1329,9 @@
       <c r="D29" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="34"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
@@ -1338,11 +1346,11 @@
       <c r="D30" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="34"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
@@ -1357,11 +1365,11 @@
       <c r="D31" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
@@ -1374,13 +1382,13 @@
       <c r="D32" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
-    </row>
-    <row r="33" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
+    </row>
+    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="6"/>
       <c r="C33" s="17" t="s">
@@ -1389,112 +1397,119 @@
       <c r="D33" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="33"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="34"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="6"/>
       <c r="C35" s="17"/>
       <c r="D35" s="23"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="34"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="6"/>
       <c r="C36" s="17"/>
       <c r="D36" s="23"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="33"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="34"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="6"/>
       <c r="C37" s="17"/>
       <c r="D37" s="23"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="34"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="6"/>
       <c r="C38" s="17"/>
       <c r="D38" s="23"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="34"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="6"/>
       <c r="C39" s="17"/>
       <c r="D39" s="23"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="34"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="6"/>
       <c r="C40" s="17"/>
       <c r="D40" s="23"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="6"/>
       <c r="C41" s="17"/>
       <c r="D41" s="23"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="32"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="6"/>
       <c r="C42" s="17"/>
       <c r="D42" s="23"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="32"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="34"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="6"/>
       <c r="C43" s="17"/>
       <c r="D43" s="23"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="32"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="6"/>
       <c r="C44" s="17"/>
       <c r="D44" s="23"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="33"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="32"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="34"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="7"/>
       <c r="C45" s="18"/>
@@ -1503,7 +1518,7 @@
       <c r="F45" s="27"/>
       <c r="G45" s="27"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="8"/>
       <c r="C46" s="19"/>
@@ -1512,7 +1527,7 @@
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="8"/>
       <c r="C47" s="19"/>
@@ -1521,7 +1536,7 @@
       <c r="F47" s="28"/>
       <c r="G47" s="28"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="8"/>
       <c r="C48" s="19"/>

</xml_diff>

<commit_message>
Erreur ajout utilisateur ds la BD
Fonctionne a la maison, pas en cours
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
   <si>
     <t>Personne</t>
   </si>
@@ -240,6 +240,24 @@
   </si>
   <si>
     <t>Les exceptions ne sont pas encore gérées</t>
+  </si>
+  <si>
+    <t>Création d'une application client serveur</t>
+  </si>
+  <si>
+    <t>Ajout d'un utilisateur ds la base de données</t>
+  </si>
+  <si>
+    <t>2-3h ?</t>
+  </si>
+  <si>
+    <t>L'ajout de l'utilisateur fonctionne</t>
+  </si>
+  <si>
+    <t>Résolution de probleme concernant l'ajout de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Je n'arrive toujours pas à ajouter l'utilisateur dans la base de donnée alors que ca fonctionnait chez moi… Probleme a résoudre !</t>
   </si>
 </sst>
 </file>
@@ -845,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:G35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1445,30 +1463,52 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="32"/>
+    <row r="36" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="5">
+        <v>43163</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>75</v>
+      </c>
       <c r="F36" s="33"/>
       <c r="G36" s="34"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+    <row r="37" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>58</v>
+      </c>
       <c r="B37" s="6"/>
-      <c r="C37" s="17"/>
+      <c r="C37" s="17" t="s">
+        <v>73</v>
+      </c>
       <c r="D37" s="23"/>
       <c r="E37" s="32"/>
       <c r="F37" s="33"/>
       <c r="G37" s="34"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="32"/>
+      <c r="B38" s="5">
+        <v>43164</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>77</v>
+      </c>
       <c r="F38" s="33"/>
       <c r="G38" s="34"/>
     </row>
@@ -1638,16 +1678,27 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1660,27 +1711,16 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Affichage demandes contact envoyees
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
   <si>
     <t>Personne</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>Mettre a jour la liste de demandes envoyées</t>
+  </si>
+  <si>
+    <t>Les demandes envoyées s'affichent correctement dans la liste</t>
   </si>
 </sst>
 </file>
@@ -636,6 +639,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -645,6 +669,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -662,36 +695,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48:G48"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -992,29 +995,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1030,11 +1033,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1049,11 +1052,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1068,11 +1071,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1087,11 +1090,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1106,11 +1109,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1125,11 +1128,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1144,11 +1147,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1163,11 +1166,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1185,11 +1188,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1204,11 +1207,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1223,11 +1226,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1240,11 +1243,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1257,11 +1260,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1274,11 +1277,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1291,11 +1294,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1308,11 +1311,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1325,11 +1328,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1342,11 +1345,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1359,9 +1362,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1374,9 +1377,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1389,9 +1392,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1404,11 +1407,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1421,9 +1424,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1436,9 +1439,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1449,9 +1452,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1462,9 +1465,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1479,11 +1482,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1498,11 +1501,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1515,11 +1518,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1530,11 +1533,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1546,9 +1549,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="33"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1562,11 +1565,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1582,11 +1585,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1597,9 +1600,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="26"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="33"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1612,11 +1615,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="25"/>
-      <c r="G38" s="26"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1631,11 +1634,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1648,11 +1651,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="26"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1667,11 +1670,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1686,11 +1689,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="26"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1715,11 +1718,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="33"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1732,19 +1735,19 @@
       <c r="O43" s="21"/>
     </row>
     <row r="44" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
-      <c r="B44" s="34">
+      <c r="A44" s="24"/>
+      <c r="B44" s="25">
         <v>43167</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="39"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1755,9 +1758,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="42"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1768,9 +1771,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="42"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="30"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1781,11 +1784,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="30"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1796,81 +1799,87 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="28"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="30"/>
+    </row>
+    <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
+      <c r="B49" s="5">
+        <v>43168</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="30"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="B50" s="6"/>
       <c r="C50" s="13"/>
       <c r="D50" s="17"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="30"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="6"/>
       <c r="C51" s="13"/>
       <c r="D51" s="17"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="30"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="6"/>
       <c r="C52" s="13"/>
       <c r="D52" s="17"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="42"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="30"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="6"/>
       <c r="C53" s="13"/>
       <c r="D53" s="17"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="42"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="30"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="6"/>
       <c r="C54" s="13"/>
       <c r="D54" s="17"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="42"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="30"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="6"/>
       <c r="C55" s="13"/>
       <c r="D55" s="17"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="42"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="30"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="6"/>
       <c r="C56" s="13"/>
       <c r="D56" s="17"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="42"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="30"/>
     </row>
     <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
       <c r="A1048576" s="7" t="s">
@@ -1882,39 +1891,16 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1927,16 +1913,39 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gestion des contacts (sauf modification)
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ProjetProgrammation\Chat\Documentation\Planification_JournalDeTravail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
   <si>
     <t>Personne</t>
   </si>
@@ -324,12 +324,21 @@
   </si>
   <si>
     <t>Les demandes envoyées s'affichent correctement dans la liste</t>
+  </si>
+  <si>
+    <t>Gestion des contacts</t>
+  </si>
+  <si>
+    <t>260min</t>
+  </si>
+  <si>
+    <t>Reste la modification du contact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -652,6 +661,42 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -659,42 +704,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,11 +984,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49:G49"/>
+      <selection activeCell="E50" sqref="E50:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -995,29 +1004,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1033,11 +1042,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1052,11 +1061,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1071,11 +1080,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1090,11 +1099,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1109,11 +1118,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1128,11 +1137,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1147,11 +1156,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1166,11 +1175,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1188,11 +1197,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1207,11 +1216,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1226,11 +1235,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1243,11 +1252,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1260,11 +1269,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1277,11 +1286,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1294,11 +1303,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1311,11 +1320,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1328,11 +1337,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1345,11 +1354,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1362,9 +1371,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1377,9 +1386,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="30"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1392,9 +1401,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1407,11 +1416,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1424,9 +1433,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1439,9 +1448,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1452,9 +1461,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="30"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1465,9 +1474,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1482,11 +1491,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1501,11 +1510,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1518,11 +1527,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1533,11 +1542,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1549,9 +1558,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="30"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1565,11 +1574,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="30"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1585,11 +1594,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="32"/>
-      <c r="G36" s="33"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="30"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1600,9 +1609,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="30"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1615,11 +1624,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="30"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1634,11 +1643,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1651,11 +1660,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1670,11 +1679,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="30"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1689,11 +1698,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="30"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1718,11 +1727,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="30"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1745,9 +1754,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="34"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="36"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="39"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1758,9 +1767,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="30"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="42"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1771,9 +1780,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="30"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="42"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1784,11 +1793,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="29"/>
-      <c r="G47" s="30"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1799,9 +1808,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="30"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1814,72 +1823,80 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="30"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="30"/>
+      <c r="B50" s="5">
+        <v>43169</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="6"/>
       <c r="C51" s="13"/>
       <c r="D51" s="17"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="30"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="42"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="6"/>
       <c r="C52" s="13"/>
       <c r="D52" s="17"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="30"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="42"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="6"/>
       <c r="C53" s="13"/>
       <c r="D53" s="17"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="30"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="42"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="6"/>
       <c r="C54" s="13"/>
       <c r="D54" s="17"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="30"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="42"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="6"/>
       <c r="C55" s="13"/>
       <c r="D55" s="17"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="30"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="42"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="6"/>
       <c r="C56" s="13"/>
       <c r="D56" s="17"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="30"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="42"/>
     </row>
     <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
       <c r="A1048576" s="7" t="s">
@@ -1891,16 +1908,39 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1913,39 +1953,16 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Contact - Modifier - Nettoyage code actionUtilisateur
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
   <si>
     <t>Personne</t>
   </si>
@@ -333,6 +333,15 @@
   </si>
   <si>
     <t>Reste la modification du contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification des contacts </t>
+  </si>
+  <si>
+    <t>Nettoyage code Serveur</t>
+  </si>
+  <si>
+    <t>Reste a nettoyer la partie BD et le client</t>
   </si>
 </sst>
 </file>
@@ -661,6 +670,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,6 +687,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -686,24 +713,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,7 +997,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50:G50"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1004,29 +1013,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1042,11 +1051,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1061,11 +1070,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1080,11 +1089,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1099,11 +1108,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1118,11 +1127,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1137,11 +1146,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1156,11 +1165,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1175,11 +1184,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1197,11 +1206,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1216,11 +1225,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1235,11 +1244,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1252,11 +1261,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1269,11 +1278,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1286,11 +1295,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1303,11 +1312,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="30"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1320,11 +1329,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1337,11 +1346,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1354,11 +1363,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1371,9 +1380,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1386,9 +1395,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1401,9 +1410,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1416,11 +1425,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1433,9 +1442,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1448,9 +1457,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1461,9 +1470,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1474,9 +1483,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1491,11 +1500,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1510,11 +1519,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1527,11 +1536,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1542,11 +1551,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1558,9 +1567,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="33"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1574,11 +1583,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1594,11 +1603,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="30"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1609,9 +1618,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="33"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1624,11 +1633,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="29"/>
-      <c r="G38" s="30"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1643,11 +1652,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="30"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1660,11 +1669,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="29"/>
-      <c r="G40" s="30"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1679,11 +1688,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E41" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="29"/>
-      <c r="G41" s="30"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1698,11 +1707,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="29"/>
-      <c r="G42" s="30"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1727,11 +1736,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="30"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="33"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1754,9 +1763,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="39"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1767,9 +1776,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="42"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1780,9 +1789,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="42"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="30"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1793,11 +1802,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="30"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1808,9 +1817,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="30"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1823,9 +1832,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="30"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
@@ -1838,65 +1847,77 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="30"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42"/>
+      <c r="B51" s="5">
+        <v>43170</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="30"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="42"/>
+      <c r="C52" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F52" s="29"/>
+      <c r="G52" s="30"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="6"/>
       <c r="C53" s="13"/>
       <c r="D53" s="17"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="42"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="30"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="6"/>
       <c r="C54" s="13"/>
       <c r="D54" s="17"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="42"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="30"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="6"/>
       <c r="C55" s="13"/>
       <c r="D55" s="17"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="42"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="30"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="6"/>
       <c r="C56" s="13"/>
       <c r="D56" s="17"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="42"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="30"/>
     </row>
     <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
       <c r="A1048576" s="7" t="s">
@@ -1908,39 +1929,16 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1953,16 +1951,39 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commencé envoi demande discussion
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ProjetProgrammation\Chat\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
   <si>
     <t>Personne</t>
   </si>
@@ -342,12 +342,18 @@
   </si>
   <si>
     <t>Reste a nettoyer la partie BD et le client</t>
+  </si>
+  <si>
+    <t>Nettoyage code ConnexionBD</t>
+  </si>
+  <si>
+    <t>Commencement coder création de discussion, envoi de demande de disucssion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -670,6 +676,42 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -677,42 +719,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,11 +999,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1013,29 +1019,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1051,11 +1057,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1070,11 +1076,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1089,11 +1095,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1108,11 +1114,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1127,11 +1133,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1146,11 +1152,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1165,11 +1171,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1184,11 +1190,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1206,11 +1212,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1225,11 +1231,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1244,11 +1250,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1261,11 +1267,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1278,11 +1284,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1295,11 +1301,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1312,11 +1318,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1329,11 +1335,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1346,11 +1352,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1363,11 +1369,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1380,9 +1386,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1395,9 +1401,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="30"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1410,9 +1416,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1425,11 +1431,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1442,9 +1448,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1457,9 +1463,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1470,9 +1476,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="30"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1483,9 +1489,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1500,11 +1506,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1519,11 +1525,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1536,11 +1542,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1551,11 +1557,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1567,9 +1573,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="30"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1583,11 +1589,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="30"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1603,11 +1609,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="32"/>
-      <c r="G36" s="33"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="30"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1618,9 +1624,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="30"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1633,11 +1639,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="30"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1652,11 +1658,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1669,11 +1675,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1688,11 +1694,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="30"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1707,11 +1713,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="30"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1736,11 +1742,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="30"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1763,9 +1769,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="34"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="36"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="39"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1776,9 +1782,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="30"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="42"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1789,9 +1795,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="30"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="42"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1802,11 +1808,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="29"/>
-      <c r="G47" s="30"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1817,9 +1823,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="30"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1832,12 +1838,14 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="30"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+      <c r="A50" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="B50" s="5">
         <v>43169</v>
       </c>
@@ -1847,14 +1855,16 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="30"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
+      <c r="A51" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="B51" s="5">
         <v>43170</v>
       </c>
@@ -1864,9 +1874,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="30"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="42"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -1877,47 +1887,59 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="29"/>
-      <c r="G52" s="30"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="42"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="30"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="5">
+        <v>43171</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" s="40"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="42"/>
+    </row>
+    <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="30"/>
+      <c r="B54" s="5">
+        <v>43172</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="40"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="42"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="6"/>
       <c r="C55" s="13"/>
       <c r="D55" s="17"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="30"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="42"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="6"/>
       <c r="C56" s="13"/>
       <c r="D56" s="17"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="30"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="42"/>
     </row>
     <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
       <c r="A1048576" s="7" t="s">
@@ -1929,16 +1951,39 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1951,39 +1996,16 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creation Discussion et participationDiscussion
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ProjetProgrammation\Chat\Documentation\Planification_JournalDeTravail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313FEA06-9E6E-4253-99DF-8AF3E29C9AA2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="111">
   <si>
     <t>Personne</t>
   </si>
@@ -348,12 +349,21 @@
   </si>
   <si>
     <t>Commencement coder création de discussion, envoi de demande de disucssion</t>
+  </si>
+  <si>
+    <t>Créer discussion + créer participation a la discussion</t>
+  </si>
+  <si>
+    <t>120min</t>
+  </si>
+  <si>
+    <t>La discussion se crée, les participants a la discussion s'ajoutent dans la base de données. Reste a ajouter la discussion pour le createur et les demandes pour les participants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -676,6 +686,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -684,6 +703,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -701,24 +729,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,11 +1009,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1014,34 +1024,34 @@
     <col min="4" max="4" width="14.5" style="14" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="18" customWidth="1"/>
     <col min="6" max="6" width="7.125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="32.25" style="18" customWidth="1"/>
+    <col min="7" max="7" width="39.75" style="18" customWidth="1"/>
     <col min="8" max="8" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1057,11 +1067,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1076,11 +1086,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1095,11 +1105,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1114,11 +1124,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1133,11 +1143,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1152,11 +1162,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1171,11 +1181,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1190,11 +1200,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1212,11 +1222,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1231,11 +1241,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1250,11 +1260,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1267,11 +1277,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1284,11 +1294,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1301,11 +1311,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1318,11 +1328,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="30"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1335,11 +1345,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1352,11 +1362,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1369,11 +1379,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1386,9 +1396,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1401,9 +1411,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1416,9 +1426,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1431,11 +1441,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1448,9 +1458,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1463,9 +1473,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1476,9 +1486,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1489,9 +1499,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1506,11 +1516,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1525,11 +1535,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1542,11 +1552,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1557,11 +1567,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1573,9 +1583,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="33"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1589,11 +1599,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1609,11 +1619,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="30"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1624,9 +1634,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="33"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1639,11 +1649,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="29"/>
-      <c r="G38" s="30"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1658,11 +1668,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="30"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1675,11 +1685,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="29"/>
-      <c r="G40" s="30"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1694,11 +1704,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E41" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="29"/>
-      <c r="G41" s="30"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1713,11 +1723,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="29"/>
-      <c r="G42" s="30"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1742,11 +1752,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="30"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="33"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1769,9 +1779,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="39"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1782,9 +1792,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="42"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1795,9 +1805,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="42"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="30"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1808,11 +1818,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="30"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1823,9 +1833,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="30"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1838,9 +1848,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="30"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -1855,11 +1865,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="30"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -1874,9 +1884,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="40"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="30"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -1887,11 +1897,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="E52" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="41"/>
-      <c r="G52" s="42"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="30"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -1904,9 +1914,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="40"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="42"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="30"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -1919,27 +1929,37 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="40"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="42"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="42"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="30"/>
+    </row>
+    <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="5">
+        <v>43172</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="32"/>
+      <c r="G55" s="33"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="6"/>
       <c r="C56" s="13"/>
       <c r="D56" s="17"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="42"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="30"/>
     </row>
     <row r="1048576" spans="1:1 16384:16384" x14ac:dyDescent="0.25">
       <c r="A1048576" s="7" t="s">
@@ -1951,39 +1971,16 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
@@ -1996,16 +1993,39 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajouter Message dans BD - Debut actualisation messages
Problème avec Timer
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="122">
   <si>
     <t>Personne</t>
   </si>
@@ -378,6 +378,18 @@
   </si>
   <si>
     <t>Affichage discussion, suppression demandes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No overload for "methode" matches delegate 'ElapsedEventHandler' </t>
+  </si>
+  <si>
+    <t>Ajouter un message ds la BD</t>
+  </si>
+  <si>
+    <t>25min</t>
+  </si>
+  <si>
+    <t>Creation d'un timer pour l'actualisation des messages envoyés</t>
   </si>
 </sst>
 </file>
@@ -745,6 +757,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,15 +801,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -779,33 +818,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60:G60"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61:G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1106,29 +1118,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="47" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1144,11 +1156,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1163,11 +1175,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1856,9 +1868,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="53"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="50"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1869,9 +1881,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="54"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="56"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="47"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1882,9 +1894,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="54"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="56"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="47"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1895,11 +1907,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="54" t="s">
+      <c r="E47" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="55"/>
-      <c r="G47" s="56"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="47"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1910,9 +1922,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="54"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="56"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="47"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1925,9 +1937,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="54"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="56"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="47"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -1942,11 +1954,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="54" t="s">
+      <c r="E50" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="55"/>
-      <c r="G50" s="56"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="47"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -1961,9 +1973,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="54"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="56"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="47"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -1974,11 +1986,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="54" t="s">
+      <c r="E52" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="55"/>
-      <c r="G52" s="56"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="47"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -1991,9 +2003,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="54"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="56"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="47"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2006,9 +2018,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="54"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="56"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="47"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2055,9 +2067,9 @@
       <c r="D57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="57"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="59"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
     </row>
     <row r="58" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
@@ -2070,11 +2082,11 @@
       <c r="D58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="57" t="s">
+      <c r="E58" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="58"/>
-      <c r="G58" s="59"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="41"/>
     </row>
     <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
@@ -2087,11 +2099,11 @@
       <c r="D59" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="39" t="s">
+      <c r="E59" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="F59" s="40"/>
-      <c r="G59" s="41"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="53"/>
     </row>
     <row r="60" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="28"/>
@@ -2104,27 +2116,39 @@
       <c r="D60" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="57"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="59"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
-      <c r="B61" s="29"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="38">
+        <v>43178</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" s="39"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
+    </row>
+    <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
       <c r="B62" s="29"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
+      <c r="C62" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62" s="40"/>
+      <c r="G62" s="41"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
@@ -4745,32 +4769,28 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
+  <mergeCells count="61">
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E34:G34"/>
@@ -4784,27 +4804,33 @@
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
     <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Début affichage message conversation
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="124">
   <si>
     <t>Personne</t>
   </si>
@@ -390,6 +390,12 @@
   </si>
   <si>
     <t>Creation d'un timer pour l'actualisation des messages envoyés</t>
+  </si>
+  <si>
+    <t>Afficher les messages lors d'une discussion/afficher les nouveaux messages</t>
+  </si>
+  <si>
+    <t>Résolution du bug ci-dessus. L'affichage des messages focntionne pour une conversation mais pas pour une autre ??</t>
   </si>
 </sst>
 </file>
@@ -774,6 +780,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -783,15 +816,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -799,24 +823,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1102,7 +1108,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61:G61"/>
+      <selection activeCell="D62" activeCellId="1" sqref="E63:G63 D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1118,29 +1124,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1156,11 +1162,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1175,11 +1181,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1868,9 +1874,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="48"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="50"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="53"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1881,9 +1887,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="47"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="56"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1894,9 +1900,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="45"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="47"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="56"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1907,11 +1913,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="45" t="s">
+      <c r="E47" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="46"/>
-      <c r="G47" s="47"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="56"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1922,9 +1928,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="45"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="47"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="56"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1937,9 +1943,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="45"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="47"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="56"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -1954,11 +1960,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="45" t="s">
+      <c r="E50" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="46"/>
-      <c r="G50" s="47"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="56"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -1973,9 +1979,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="45"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="47"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="56"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -1986,11 +1992,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="45" t="s">
+      <c r="E52" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="46"/>
-      <c r="G52" s="47"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="56"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -2003,9 +2009,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="45"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="47"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="56"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2018,9 +2024,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="45"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="47"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="56"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2099,11 +2105,11 @@
       <c r="D59" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="51" t="s">
+      <c r="E59" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="F59" s="52"/>
-      <c r="G59" s="53"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="59"/>
     </row>
     <row r="60" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="28"/>
@@ -2150,14 +2156,22 @@
       <c r="F62" s="40"/>
       <c r="G62" s="41"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
-      <c r="B63" s="29"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="32"/>
+      <c r="B63" s="38">
+        <v>43151</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="58"/>
+      <c r="G63" s="59"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="28"/>
@@ -4769,13 +4783,43 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E61:G61"/>
+  <mergeCells count="62">
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="A1:C2"/>
@@ -4786,6 +4830,12 @@
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E61:G61"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E18:G18"/>
@@ -4796,41 +4846,6 @@
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E59:G59"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout/Suppression utilisateur discussion - archivage discussion
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="128">
   <si>
     <t>Personne</t>
   </si>
@@ -396,6 +396,18 @@
   </si>
   <si>
     <t>Résolution du bug ci-dessus. L'affichage des messages focntionne pour une conversation mais pas pour une autre ??</t>
+  </si>
+  <si>
+    <t>Resolution d'un bug ou les messages ne s'affichaient pas en entier</t>
+  </si>
+  <si>
+    <t>Ajout/Suppresion de membres dans la discussion</t>
+  </si>
+  <si>
+    <t>Archivage des discussions</t>
+  </si>
+  <si>
+    <t>Reste a pouvoir les reimporter</t>
   </si>
 </sst>
 </file>
@@ -763,6 +775,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -780,6 +801,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -796,33 +835,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1107,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="D62" activeCellId="1" sqref="E63:G63 D62"/>
+    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66:G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1124,29 +1136,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="47" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1162,11 +1174,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1181,11 +1193,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1200,11 +1212,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1219,11 +1231,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1238,11 +1250,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1257,11 +1269,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1276,11 +1288,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1295,11 +1307,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1317,11 +1329,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="47"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1336,11 +1348,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1355,11 +1367,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1372,11 +1384,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1389,11 +1401,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1406,11 +1418,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1423,11 +1435,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1440,11 +1452,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1457,11 +1469,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1474,11 +1486,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1491,9 +1503,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="47"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1506,9 +1518,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1521,9 +1533,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1536,11 +1548,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="43"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1553,9 +1565,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1568,9 +1580,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1581,9 +1593,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1594,9 +1606,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1611,11 +1623,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1630,11 +1642,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1647,11 +1659,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1662,11 +1674,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1678,9 +1690,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1694,11 +1706,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1714,11 +1726,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="47"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1729,9 +1741,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="47"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1744,11 +1756,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="47"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1763,11 +1775,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1780,11 +1792,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="47"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1799,11 +1811,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="43"/>
-      <c r="G41" s="44"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="47"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1818,11 +1830,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1847,11 +1859,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="44"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1887,9 +1899,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="54"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="56"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="50"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1900,9 +1912,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="54"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="56"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="50"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1913,11 +1925,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="54" t="s">
+      <c r="E47" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="55"/>
-      <c r="G47" s="56"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="50"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1928,9 +1940,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="54"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="56"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="50"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1943,9 +1955,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="54"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="56"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="50"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -1960,11 +1972,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="54" t="s">
+      <c r="E50" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="55"/>
-      <c r="G50" s="56"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="50"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -1979,9 +1991,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="54"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="56"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="50"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -1992,11 +2004,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="54" t="s">
+      <c r="E52" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="55"/>
-      <c r="G52" s="56"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="50"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -2009,9 +2021,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="54"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="56"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="50"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2024,9 +2036,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="54"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="56"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="50"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2041,11 +2053,11 @@
       <c r="D55" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E55" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="47"/>
     </row>
     <row r="56" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
@@ -2058,11 +2070,11 @@
       <c r="D56" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="43"/>
-      <c r="G56" s="44"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="47"/>
     </row>
     <row r="57" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
@@ -2073,9 +2085,9 @@
       <c r="D57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="39"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="41"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="44"/>
     </row>
     <row r="58" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
@@ -2088,11 +2100,11 @@
       <c r="D58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="39" t="s">
+      <c r="E58" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="40"/>
-      <c r="G58" s="41"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="44"/>
     </row>
     <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
@@ -2105,11 +2117,11 @@
       <c r="D59" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="57" t="s">
+      <c r="E59" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="F59" s="58"/>
-      <c r="G59" s="59"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="41"/>
     </row>
     <row r="60" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="28"/>
@@ -2122,9 +2134,9 @@
       <c r="D60" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="39"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="41"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="44"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
@@ -2137,9 +2149,9 @@
       <c r="D61" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="39"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="41"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="44"/>
     </row>
     <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
@@ -2150,11 +2162,11 @@
       <c r="D62" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="39" t="s">
+      <c r="E62" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="40"/>
-      <c r="G62" s="41"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="44"/>
     </row>
     <row r="63" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
@@ -2167,38 +2179,54 @@
       <c r="D63" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E63" s="57" t="s">
+      <c r="E63" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="F63" s="58"/>
-      <c r="G63" s="59"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F63" s="40"/>
+      <c r="G63" s="41"/>
+    </row>
+    <row r="64" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A64" s="28"/>
-      <c r="B64" s="29"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="38">
+        <v>43153</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" s="39"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="41"/>
+    </row>
+    <row r="65" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A65" s="28"/>
       <c r="B65" s="29"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
+      <c r="C65" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E65" s="39"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="41"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="28"/>
       <c r="B66" s="29"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
+      <c r="C66" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F66" s="40"/>
+      <c r="G66" s="41"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
@@ -4783,54 +4811,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E62:G62"/>
+  <mergeCells count="65">
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
@@ -4846,6 +4830,53 @@
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E62:G62"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reimporter archives - test connexion avec plusieurs clients
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="131">
   <si>
     <t>Personne</t>
   </si>
@@ -408,6 +408,15 @@
   </si>
   <si>
     <t>Reste a pouvoir les reimporter</t>
+  </si>
+  <si>
+    <t>Reimporter les discussion</t>
+  </si>
+  <si>
+    <t>Test de chat avec plusieurs clients.</t>
+  </si>
+  <si>
+    <t>Cela fonctionne, mais le serveur plante lors de l'archivage. Avec l'aide de M. Ithurbide j'ai pu faire fonctionner cela. M. m'a expliqué comment faire pour que mon serveur écoute sur plusieurs ports et m'a donné plusieurs conseils pour l'ergonomie de l'application</t>
   </si>
 </sst>
 </file>
@@ -783,6 +792,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,13 +810,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -809,33 +845,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,7 +1129,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66:G66"/>
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1136,29 +1145,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1174,11 +1183,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1193,11 +1202,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1212,11 +1221,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1231,11 +1240,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1250,11 +1259,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1269,11 +1278,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="47"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1288,11 +1297,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="47"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1307,11 +1316,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1329,11 +1338,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="47"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1348,11 +1357,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="47"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1367,11 +1376,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1384,11 +1393,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1401,11 +1410,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1418,11 +1427,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1435,11 +1444,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="45" t="s">
+      <c r="E18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1452,11 +1461,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E19" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="44"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1469,11 +1478,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1486,11 +1495,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="45" t="s">
+      <c r="E21" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="47"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1503,9 +1512,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="47"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1518,9 +1527,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="47"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="44"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1533,9 +1542,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1548,11 +1557,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1565,9 +1574,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1580,9 +1589,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="44"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1593,9 +1602,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1606,9 +1615,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="45"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1623,11 +1632,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1642,11 +1651,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="46"/>
-      <c r="G31" s="47"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1659,11 +1668,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="45" t="s">
+      <c r="E32" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="47"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1674,11 +1683,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="45" t="s">
+      <c r="E33" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="46"/>
-      <c r="G33" s="47"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1690,9 +1699,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="45"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="47"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1706,11 +1715,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="46"/>
-      <c r="G35" s="47"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1726,11 +1735,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="45" t="s">
+      <c r="E36" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="46"/>
-      <c r="G36" s="47"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1741,9 +1750,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="47"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="44"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1756,11 +1765,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="45" t="s">
+      <c r="E38" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="46"/>
-      <c r="G38" s="47"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="44"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1775,11 +1784,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="45" t="s">
+      <c r="E39" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="47"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="44"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1792,11 +1801,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E40" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="46"/>
-      <c r="G40" s="47"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="44"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1811,11 +1820,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="45" t="s">
+      <c r="E41" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="46"/>
-      <c r="G41" s="47"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="44"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1830,11 +1839,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="44"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1859,11 +1868,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="46"/>
-      <c r="G43" s="47"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="44"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1886,9 +1895,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="53"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="56"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1899,9 +1908,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="48"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="50"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="59"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1912,9 +1921,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="48"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="50"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="59"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1925,11 +1934,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="48" t="s">
+      <c r="E47" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="49"/>
-      <c r="G47" s="50"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="59"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1940,9 +1949,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="50"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="59"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1955,9 +1964,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="48"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="50"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="59"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -1972,11 +1981,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="48" t="s">
+      <c r="E50" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="49"/>
-      <c r="G50" s="50"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="59"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -1991,9 +2000,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="50"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="59"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -2004,11 +2013,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="48" t="s">
+      <c r="E52" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="49"/>
-      <c r="G52" s="50"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="59"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -2021,9 +2030,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="48"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="50"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="59"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2036,9 +2045,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="48"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="50"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="59"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2053,11 +2062,11 @@
       <c r="D55" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="45" t="s">
+      <c r="E55" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="F55" s="46"/>
-      <c r="G55" s="47"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="44"/>
     </row>
     <row r="56" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
@@ -2070,11 +2079,11 @@
       <c r="D56" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="45" t="s">
+      <c r="E56" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="46"/>
-      <c r="G56" s="47"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="44"/>
     </row>
     <row r="57" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
@@ -2085,9 +2094,9 @@
       <c r="D57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="42"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="44"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="47"/>
     </row>
     <row r="58" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
@@ -2100,11 +2109,11 @@
       <c r="D58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="42" t="s">
+      <c r="E58" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="43"/>
-      <c r="G58" s="44"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="47"/>
     </row>
     <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
@@ -2134,9 +2143,9 @@
       <c r="D60" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="42"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="44"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="47"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
@@ -2149,9 +2158,9 @@
       <c r="D61" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="42"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="44"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="47"/>
     </row>
     <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
@@ -2162,11 +2171,11 @@
       <c r="D62" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="42" t="s">
+      <c r="E62" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="43"/>
-      <c r="G62" s="44"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="47"/>
     </row>
     <row r="63" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
@@ -2228,23 +2237,35 @@
       <c r="F66" s="40"/>
       <c r="G66" s="41"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
-      <c r="B67" s="29"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="32"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="38">
+        <v>43154</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" s="39"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="41"/>
+    </row>
+    <row r="68" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A68" s="28"/>
       <c r="B68" s="29"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="32"/>
+      <c r="C68" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D68" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="F68" s="40"/>
+      <c r="G68" s="41"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="28"/>
@@ -4811,7 +4832,58 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="67">
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="E64:G64"/>
     <mergeCell ref="E65:G65"/>
     <mergeCell ref="E66:G66"/>
@@ -4828,55 +4900,6 @@
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E62:G62"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Recherche discussion publique - corrections de bugs lors de création/ajout
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="141">
   <si>
     <t>Personne</t>
   </si>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>Les recherches de discussions se feront seulement sur les discussions publiques. Une liste de environ 10 categories de discussion sera proposée. Si une categorie est selectionnée, une fenetre contenant les discussions publiques correspondantes a cette categorie apparaitra. Il y aura aussi la possibilité de rechercher une discussion en tappant le nom d'une categorie. A chaque nouveau caractère rentré une liste des categories correspondants à la chaine actuelle sera proposée.</t>
+  </si>
+  <si>
+    <t>Recherche des discussion publique terminee</t>
+  </si>
+  <si>
+    <t>135min</t>
+  </si>
+  <si>
+    <t>Correction de "bugs"</t>
+  </si>
+  <si>
+    <t>On ne peut pas ajouter un contact déjà existant ou soit meme. Lorsque je recherche une discussion publique, les discussions auxquelles je participe déjà ne s'affichent pas</t>
   </si>
 </sst>
 </file>
@@ -810,6 +822,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -819,13 +840,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -836,33 +875,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1146,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71:G71"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1163,29 +1175,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1201,11 +1213,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1220,11 +1232,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1239,11 +1251,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1258,11 +1270,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1277,11 +1289,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1296,11 +1308,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="47"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1315,11 +1327,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="47"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1334,11 +1346,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1356,11 +1368,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="47"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1375,11 +1387,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="47"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1394,11 +1406,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1411,11 +1423,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1428,11 +1440,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1445,11 +1457,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1462,11 +1474,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="45" t="s">
+      <c r="E18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1479,11 +1491,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E19" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="44"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1496,11 +1508,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1513,11 +1525,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="45" t="s">
+      <c r="E21" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="47"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1530,9 +1542,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="47"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1545,9 +1557,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="47"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="44"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1560,9 +1572,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1575,11 +1587,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1592,9 +1604,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1607,9 +1619,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="44"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1620,9 +1632,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1633,9 +1645,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="45"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1650,11 +1662,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1669,11 +1681,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="46"/>
-      <c r="G31" s="47"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1686,11 +1698,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="45" t="s">
+      <c r="E32" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="47"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1701,11 +1713,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="45" t="s">
+      <c r="E33" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="46"/>
-      <c r="G33" s="47"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1717,9 +1729,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="45"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="47"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1733,11 +1745,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="46"/>
-      <c r="G35" s="47"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1753,11 +1765,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="45" t="s">
+      <c r="E36" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="46"/>
-      <c r="G36" s="47"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1768,9 +1780,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="47"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="44"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1783,11 +1795,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="45" t="s">
+      <c r="E38" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="46"/>
-      <c r="G38" s="47"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="44"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1802,11 +1814,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="45" t="s">
+      <c r="E39" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="47"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="44"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1819,11 +1831,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E40" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="46"/>
-      <c r="G40" s="47"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="44"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1838,11 +1850,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="45" t="s">
+      <c r="E41" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="46"/>
-      <c r="G41" s="47"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="44"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1857,11 +1869,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="44"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1886,11 +1898,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="46"/>
-      <c r="G43" s="47"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="44"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1913,9 +1925,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="53"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="56"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1926,9 +1938,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="48"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="50"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="59"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1939,9 +1951,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="48"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="50"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="59"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1952,11 +1964,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="48" t="s">
+      <c r="E47" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="49"/>
-      <c r="G47" s="50"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="59"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1967,9 +1979,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="50"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="59"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1982,9 +1994,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="48"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="50"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="59"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -1999,11 +2011,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="48" t="s">
+      <c r="E50" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="49"/>
-      <c r="G50" s="50"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="59"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -2018,9 +2030,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="50"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="59"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -2031,11 +2043,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="48" t="s">
+      <c r="E52" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="49"/>
-      <c r="G52" s="50"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="59"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -2048,9 +2060,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="48"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="50"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="59"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2063,9 +2075,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="48"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="50"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="59"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2080,11 +2092,11 @@
       <c r="D55" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="45" t="s">
+      <c r="E55" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="F55" s="46"/>
-      <c r="G55" s="47"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="44"/>
     </row>
     <row r="56" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
@@ -2097,11 +2109,11 @@
       <c r="D56" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="45" t="s">
+      <c r="E56" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="46"/>
-      <c r="G56" s="47"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="44"/>
     </row>
     <row r="57" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
@@ -2112,9 +2124,9 @@
       <c r="D57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="42"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="44"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="47"/>
     </row>
     <row r="58" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
@@ -2127,11 +2139,11 @@
       <c r="D58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="42" t="s">
+      <c r="E58" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="43"/>
-      <c r="G58" s="44"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="47"/>
     </row>
     <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
@@ -2161,9 +2173,9 @@
       <c r="D60" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="42"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="44"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="47"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
@@ -2176,9 +2188,9 @@
       <c r="D61" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="42"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="44"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="47"/>
     </row>
     <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
@@ -2189,11 +2201,11 @@
       <c r="D62" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="42" t="s">
+      <c r="E62" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="43"/>
-      <c r="G62" s="44"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="47"/>
     </row>
     <row r="63" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
@@ -2332,23 +2344,35 @@
       <c r="F71" s="40"/>
       <c r="G71" s="41"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A72" s="28"/>
-      <c r="B72" s="29"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="31"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="32"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="38">
+        <v>43188</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="45"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="47"/>
+    </row>
+    <row r="73" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="28"/>
       <c r="B73" s="29"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="31"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="32"/>
+      <c r="C73" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E73" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="F73" s="40"/>
+      <c r="G73" s="41"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="28"/>
@@ -4870,7 +4894,63 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="72">
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="E69:G69"/>
     <mergeCell ref="E70:G70"/>
     <mergeCell ref="E71:G71"/>
@@ -4887,60 +4967,6 @@
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactoring 10 premiers messages
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ProjetProgrammation\Chat\Documentation\Planification_JournalDeTravail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DA01E4-7407-4EB6-902E-FCEADC099257}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="144">
   <si>
     <t>Personne</t>
   </si>
@@ -447,12 +448,21 @@
   </si>
   <si>
     <t>On ne peut pas ajouter un contact déjà existant ou soit meme. Lorsque je recherche une discussion publique, les discussions auxquelles je participe déjà ne s'affichent pas</t>
+  </si>
+  <si>
+    <t>35min</t>
+  </si>
+  <si>
+    <t>Refactoring des 10 premiers "messsages"</t>
+  </si>
+  <si>
+    <t>Ajout de commentaires / Amelioration des fonctions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -814,6 +824,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -831,14 +850,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -857,24 +885,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1155,11 +1165,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="E74" sqref="E74:G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1175,29 +1185,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1213,11 +1223,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1232,11 +1242,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1251,11 +1261,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1270,11 +1280,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1289,11 +1299,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1308,11 +1318,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1327,11 +1337,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1346,11 +1356,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1368,11 +1378,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="47"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1387,11 +1397,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1406,11 +1416,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1423,11 +1433,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1440,11 +1450,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1457,11 +1467,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1474,11 +1484,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1491,11 +1501,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1508,11 +1518,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1525,11 +1535,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1542,9 +1552,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="47"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1557,9 +1567,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1572,9 +1582,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1587,11 +1597,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="43"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1604,9 +1614,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1619,9 +1629,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1632,9 +1642,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1645,9 +1655,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1662,11 +1672,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1681,11 +1691,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1698,11 +1708,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1713,11 +1723,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1729,9 +1739,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1745,11 +1755,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1765,11 +1775,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="47"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1780,9 +1790,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="47"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1795,11 +1805,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="47"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1814,11 +1824,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1831,11 +1841,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="47"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1850,11 +1860,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="43"/>
-      <c r="G41" s="44"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="47"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1869,11 +1879,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1898,11 +1908,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="44"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1925,9 +1935,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="54"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="56"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="53"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1938,9 +1948,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="57"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="59"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="50"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1951,9 +1961,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="59"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="50"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1964,11 +1974,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="59"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="50"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1979,9 +1989,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="57"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="59"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="50"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1994,9 +2004,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="57"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="59"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="50"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -2011,11 +2021,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="58"/>
-      <c r="G50" s="59"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="50"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -2030,9 +2040,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="57"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="59"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="50"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -2043,11 +2053,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="57" t="s">
+      <c r="E52" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="58"/>
-      <c r="G52" s="59"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="50"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -2060,9 +2070,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="57"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="59"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="50"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2075,9 +2085,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="57"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="59"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="50"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2092,11 +2102,11 @@
       <c r="D55" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E55" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="47"/>
     </row>
     <row r="56" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
@@ -2109,11 +2119,11 @@
       <c r="D56" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="43"/>
-      <c r="G56" s="44"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="47"/>
     </row>
     <row r="57" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
@@ -2124,9 +2134,9 @@
       <c r="D57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="45"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="47"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
     </row>
     <row r="58" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
@@ -2139,11 +2149,11 @@
       <c r="D58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="45" t="s">
+      <c r="E58" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="46"/>
-      <c r="G58" s="47"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="41"/>
     </row>
     <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
@@ -2156,11 +2166,11 @@
       <c r="D59" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="39" t="s">
+      <c r="E59" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F59" s="40"/>
-      <c r="G59" s="41"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="44"/>
     </row>
     <row r="60" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="28"/>
@@ -2173,9 +2183,9 @@
       <c r="D60" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="47"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
@@ -2188,9 +2198,9 @@
       <c r="D61" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="45"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="47"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
     </row>
     <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
@@ -2201,11 +2211,11 @@
       <c r="D62" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="45" t="s">
+      <c r="E62" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="46"/>
-      <c r="G62" s="47"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="41"/>
     </row>
     <row r="63" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
@@ -2218,11 +2228,11 @@
       <c r="D63" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E63" s="39" t="s">
+      <c r="E63" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="F63" s="40"/>
-      <c r="G63" s="41"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="44"/>
     </row>
     <row r="64" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A64" s="28"/>
@@ -2235,9 +2245,9 @@
       <c r="D64" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E64" s="39"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="41"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="44"/>
     </row>
     <row r="65" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A65" s="28"/>
@@ -2248,9 +2258,9 @@
       <c r="D65" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E65" s="39"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="41"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="44"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="28"/>
@@ -2261,11 +2271,11 @@
       <c r="D66" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="39" t="s">
+      <c r="E66" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="F66" s="40"/>
-      <c r="G66" s="41"/>
+      <c r="F66" s="43"/>
+      <c r="G66" s="44"/>
     </row>
     <row r="67" spans="1:7" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
@@ -2278,9 +2288,9 @@
       <c r="D67" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E67" s="39"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="41"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="44"/>
     </row>
     <row r="68" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A68" s="28"/>
@@ -2291,11 +2301,11 @@
       <c r="D68" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E68" s="39" t="s">
+      <c r="E68" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="F68" s="40"/>
-      <c r="G68" s="41"/>
+      <c r="F68" s="43"/>
+      <c r="G68" s="44"/>
     </row>
     <row r="69" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A69" s="28"/>
@@ -2308,9 +2318,9 @@
       <c r="D69" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E69" s="39"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="41"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="44"/>
     </row>
     <row r="70" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="28"/>
@@ -2323,11 +2333,11 @@
       <c r="D70" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="E70" s="39" t="s">
+      <c r="E70" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="F70" s="40"/>
-      <c r="G70" s="41"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="44"/>
     </row>
     <row r="71" spans="1:7" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="28"/>
@@ -2338,11 +2348,11 @@
       <c r="D71" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E71" s="39" t="s">
+      <c r="E71" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="F71" s="40"/>
-      <c r="G71" s="41"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="44"/>
     </row>
     <row r="72" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A72" s="28"/>
@@ -2355,9 +2365,9 @@
       <c r="D72" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E72" s="45"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="47"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="40"/>
+      <c r="G72" s="41"/>
     </row>
     <row r="73" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="28"/>
@@ -2368,20 +2378,28 @@
       <c r="D73" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="E73" s="39" t="s">
+      <c r="E73" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="F73" s="40"/>
-      <c r="G73" s="41"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F73" s="43"/>
+      <c r="G73" s="44"/>
+    </row>
+    <row r="74" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A74" s="28"/>
-      <c r="B74" s="29"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="32"/>
+      <c r="B74" s="38">
+        <v>43203</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E74" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="43"/>
+      <c r="G74" s="44"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="28"/>
@@ -4894,66 +4912,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
+  <mergeCells count="73">
+    <mergeCell ref="E74:G74"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
@@ -4967,6 +4927,65 @@
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fin ecriture tests, chatApplication commenté jusqu' a frmEnregistrement
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBA6E3B-F964-4402-A9CE-4235348A649B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BE094C-F5D3-401B-9A79-C65B29E72A14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="152">
   <si>
     <t>Personne</t>
   </si>
@@ -469,6 +469,18 @@
   </si>
   <si>
     <t xml:space="preserve">Le code du serveur est nettoyé et commenté. Reste le code du client a commenter correctement. </t>
+  </si>
+  <si>
+    <t>Debut écriture des tests</t>
+  </si>
+  <si>
+    <t>150min</t>
+  </si>
+  <si>
+    <t>Fin ecriture des tests + commentaires ChatApplication</t>
+  </si>
+  <si>
+    <t>Commentaires fait jusqu' a frmEnregistrement</t>
   </si>
 </sst>
 </file>
@@ -844,6 +856,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -853,14 +874,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -879,24 +909,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76:G76"/>
+    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78:G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1197,29 +1209,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1235,11 +1247,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1254,11 +1266,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1273,11 +1285,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1292,11 +1304,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1311,11 +1323,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1330,11 +1342,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1349,11 +1361,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1368,11 +1380,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1390,11 +1402,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="47"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1409,11 +1421,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1428,11 +1440,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1445,11 +1457,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1462,11 +1474,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1479,11 +1491,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1496,11 +1508,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1513,11 +1525,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1530,11 +1542,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1547,11 +1559,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1564,9 +1576,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="47"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1579,9 +1591,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1594,9 +1606,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1609,11 +1621,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="43"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1626,9 +1638,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1641,9 +1653,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1654,9 +1666,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1667,9 +1679,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1684,11 +1696,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1703,11 +1715,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1720,11 +1732,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1735,11 +1747,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1751,9 +1763,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1767,11 +1779,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1787,11 +1799,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="47"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1802,9 +1814,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="47"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1817,11 +1829,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="47"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1836,11 +1848,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1853,11 +1865,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="47"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1872,11 +1884,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="43"/>
-      <c r="G41" s="44"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="47"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1891,11 +1903,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1920,11 +1932,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="44"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1947,9 +1959,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="54"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="56"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="53"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1960,9 +1972,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="57"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="59"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="50"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1973,9 +1985,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="59"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="50"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1986,11 +1998,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="59"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="50"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -2001,9 +2013,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="57"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="59"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="50"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -2016,9 +2028,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="57"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="59"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="50"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -2033,11 +2045,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="58"/>
-      <c r="G50" s="59"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="50"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -2052,9 +2064,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="57"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="59"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="50"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -2065,11 +2077,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="57" t="s">
+      <c r="E52" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="58"/>
-      <c r="G52" s="59"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="50"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -2082,9 +2094,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="57"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="59"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="50"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2097,9 +2109,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="57"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="59"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="50"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2114,11 +2126,11 @@
       <c r="D55" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E55" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="47"/>
     </row>
     <row r="56" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
@@ -2131,11 +2143,11 @@
       <c r="D56" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="43"/>
-      <c r="G56" s="44"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="47"/>
     </row>
     <row r="57" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
@@ -2146,9 +2158,9 @@
       <c r="D57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="45"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="47"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="44"/>
     </row>
     <row r="58" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
@@ -2161,11 +2173,11 @@
       <c r="D58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="45" t="s">
+      <c r="E58" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="46"/>
-      <c r="G58" s="47"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="44"/>
     </row>
     <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
@@ -2195,9 +2207,9 @@
       <c r="D60" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="47"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="44"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
@@ -2210,9 +2222,9 @@
       <c r="D61" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="45"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="47"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="44"/>
     </row>
     <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
@@ -2223,11 +2235,11 @@
       <c r="D62" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="45" t="s">
+      <c r="E62" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="46"/>
-      <c r="G62" s="47"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="44"/>
     </row>
     <row r="63" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
@@ -2377,9 +2389,9 @@
       <c r="D72" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E72" s="45"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="47"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="43"/>
+      <c r="G72" s="44"/>
     </row>
     <row r="73" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="28"/>
@@ -2447,21 +2459,35 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="28"/>
-      <c r="B77" s="29"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="32"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="38">
+        <v>43147</v>
+      </c>
+      <c r="C77" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E77" s="39"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="41"/>
+    </row>
+    <row r="78" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="28"/>
-      <c r="B78" s="29"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="32"/>
+      <c r="B78" s="38">
+        <v>43147</v>
+      </c>
+      <c r="C78" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="D78" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E78" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="F78" s="40"/>
+      <c r="G78" s="41"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="28"/>
@@ -4938,67 +4964,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E74:G74"/>
+  <mergeCells count="77">
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
@@ -5014,6 +4982,66 @@
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E74:G74"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Réalisation des tests- début
</commit_message>
<xml_diff>
--- a/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
+++ b/Documentation/Planification_JournalDeTravail/Journal de travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ProjetProgrammation\Chat\Documentation\Planification_JournalDeTravail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chat-Application\Documentation\Planification_JournalDeTravail\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399EC1F6-61DD-499E-8A8A-99A3FCDC7A63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="157">
   <si>
     <t>Personne</t>
   </si>
@@ -489,12 +490,18 @@
   </si>
   <si>
     <t>Diagramme de classe</t>
+  </si>
+  <si>
+    <t>Début réalisation des tests</t>
+  </si>
+  <si>
+    <t>Certains bugs trouvés sont facilement corrigible, d'autres dépendent de la facon dont j'ai choisi de transmettre les informations entre le client et le serveur donc sont plus difficilement corrigibles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -864,6 +871,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -873,14 +889,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -899,24 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1197,11 +1204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B71" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1217,29 +1224,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="XFD1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8 16384:16384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:8 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8 16384:16384" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1255,11 +1262,11 @@
       <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1274,11 +1281,11 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1293,11 +1300,11 @@
       <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1312,11 +1319,11 @@
       <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
     </row>
     <row r="8" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1331,11 +1338,11 @@
       <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:8 16384:16384" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -1350,11 +1357,11 @@
       <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
     </row>
     <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1369,11 +1376,11 @@
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
     </row>
     <row r="11" spans="1:8 16384:16384" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1388,11 +1395,11 @@
       <c r="D11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -1410,11 +1417,11 @@
       <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="47"/>
     </row>
     <row r="13" spans="1:8 16384:16384" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1429,11 +1436,11 @@
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47"/>
     </row>
     <row r="14" spans="1:8 16384:16384" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1448,11 +1455,11 @@
       <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:8 16384:16384" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1465,11 +1472,11 @@
       <c r="D15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
     </row>
     <row r="16" spans="1:8 16384:16384" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1482,11 +1489,11 @@
       <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1499,11 +1506,11 @@
       <c r="D17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1516,11 +1523,11 @@
       <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1533,11 +1540,11 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1550,11 +1557,11 @@
       <c r="D20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1567,11 +1574,11 @@
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -1584,9 +1591,9 @@
       <c r="D22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="47"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1599,9 +1606,9 @@
       <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -1614,9 +1621,9 @@
       <c r="D24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
     </row>
     <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
@@ -1629,11 +1636,11 @@
       <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="43"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -1646,9 +1653,9 @@
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1661,9 +1668,9 @@
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1674,9 +1681,9 @@
       <c r="D28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
@@ -1687,9 +1694,9 @@
       <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1704,11 +1711,11 @@
       <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
     </row>
     <row r="31" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -1723,11 +1730,11 @@
       <c r="D31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
     </row>
     <row r="32" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -1740,11 +1747,11 @@
       <c r="D32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
     </row>
     <row r="33" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -1755,11 +1762,11 @@
       <c r="D33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -1771,9 +1778,9 @@
       <c r="D34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1787,11 +1794,11 @@
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1807,11 +1814,11 @@
       <c r="D36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="47"/>
     </row>
     <row r="37" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1822,9 +1829,9 @@
         <v>72</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="47"/>
     </row>
     <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -1837,11 +1844,11 @@
       <c r="D38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="47"/>
     </row>
     <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -1856,11 +1863,11 @@
       <c r="D39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -1873,11 +1880,11 @@
       <c r="D40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="47"/>
     </row>
     <row r="41" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1892,11 +1899,11 @@
       <c r="D41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="43"/>
-      <c r="G41" s="44"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="47"/>
     </row>
     <row r="42" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -1911,11 +1918,11 @@
       <c r="D42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
       <c r="H42" s="22" t="s">
         <v>86</v>
       </c>
@@ -1940,11 +1947,11 @@
       <c r="D43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="44"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="21" t="s">
         <v>87</v>
       </c>
@@ -1967,9 +1974,9 @@
       <c r="D44" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="54"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="56"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="53"/>
     </row>
     <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
@@ -1980,9 +1987,9 @@
       <c r="D45" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="57"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="59"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="50"/>
     </row>
     <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
@@ -1993,9 +2000,9 @@
       <c r="D46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="59"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="50"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -2006,11 +2013,11 @@
       <c r="D47" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="59"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="50"/>
     </row>
     <row r="48" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -2021,9 +2028,9 @@
       <c r="D48" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="57"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="59"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="50"/>
     </row>
     <row r="49" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -2036,9 +2043,9 @@
       <c r="D49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="57"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="59"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="50"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
@@ -2053,11 +2060,11 @@
       <c r="D50" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="58"/>
-      <c r="G50" s="59"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="50"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
@@ -2072,9 +2079,9 @@
       <c r="D51" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="57"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="59"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="50"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
@@ -2085,11 +2092,11 @@
       <c r="D52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="57" t="s">
+      <c r="E52" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="58"/>
-      <c r="G52" s="59"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="50"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
@@ -2102,9 +2109,9 @@
       <c r="D53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="57"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="59"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="50"/>
     </row>
     <row r="54" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
@@ -2117,9 +2124,9 @@
       <c r="D54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="57"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="59"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="50"/>
     </row>
     <row r="55" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
@@ -2134,11 +2141,11 @@
       <c r="D55" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E55" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="47"/>
     </row>
     <row r="56" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
@@ -2151,11 +2158,11 @@
       <c r="D56" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="43"/>
-      <c r="G56" s="44"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="47"/>
     </row>
     <row r="57" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
@@ -2166,9 +2173,9 @@
       <c r="D57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="45"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="47"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="44"/>
     </row>
     <row r="58" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
@@ -2181,11 +2188,11 @@
       <c r="D58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="45" t="s">
+      <c r="E58" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="46"/>
-      <c r="G58" s="47"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="44"/>
     </row>
     <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
@@ -2215,9 +2222,9 @@
       <c r="D60" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="47"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="44"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
@@ -2230,9 +2237,9 @@
       <c r="D61" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="45"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="47"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="44"/>
     </row>
     <row r="62" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
@@ -2243,11 +2250,11 @@
       <c r="D62" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="45" t="s">
+      <c r="E62" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="46"/>
-      <c r="G62" s="47"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="44"/>
     </row>
     <row r="63" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
@@ -2397,9 +2404,9 @@
       <c r="D72" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E72" s="45"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="47"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="43"/>
+      <c r="G72" s="44"/>
     </row>
     <row r="73" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="28"/>
@@ -2523,20 +2530,28 @@
       <c r="D80" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E80" s="45" t="s">
+      <c r="E80" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="F80" s="46"/>
-      <c r="G80" s="47"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F80" s="43"/>
+      <c r="G80" s="44"/>
+    </row>
+    <row r="81" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="28"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="32"/>
+      <c r="B81" s="38">
+        <v>43148</v>
+      </c>
+      <c r="C81" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="D81" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E81" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F81" s="40"/>
+      <c r="G81" s="41"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="28"/>
@@ -4986,7 +5001,71 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="80">
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
     <mergeCell ref="E79:G79"/>
     <mergeCell ref="E80:G80"/>
     <mergeCell ref="E75:G75"/>
@@ -5003,69 +5082,6 @@
     <mergeCell ref="E67:G67"/>
     <mergeCell ref="E68:G68"/>
     <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E31:G31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>